<commit_message>
Updated the tasks and made progress on the database setup for notes.
</commit_message>
<xml_diff>
--- a/Documents/Features & User Stories.xlsx
+++ b/Documents/Features & User Stories.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Kyle/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Kyle/Documents/Development/CSE110App/ToDoList/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="55">
   <si>
     <t>Feature</t>
   </si>
@@ -124,9 +124,6 @@
     <t>As a user, I need a performance tab so that I can measure my preformance metrics.</t>
   </si>
   <si>
-    <t>As a developer, we need a table set up in SQL light so that we can save and delete data for tasks.</t>
-  </si>
-  <si>
     <t>Misc/ Security/ Database</t>
   </si>
   <si>
@@ -167,6 +164,54 @@
   </si>
   <si>
     <t>As a user, I need a view for modifying tasks so that I can edit tasks.</t>
+  </si>
+  <si>
+    <t>As a user, I need an alert that lets me know when I'm leaving the create task page if the form is dirty.</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>As a developer, we need a task table set up in SQL light so that we can save and delete data for tasks.</t>
+  </si>
+  <si>
+    <t>As a developer, we need a notebook table set up in SQL light so that we can save and delete data for notes.</t>
+  </si>
+  <si>
+    <t>As a developer, I need to implement the new tab UI.</t>
+  </si>
+  <si>
+    <t>Person Assigned</t>
+  </si>
+  <si>
+    <t>As a developer, we create excel file with the database file so that we have a visual representation of the db.</t>
+  </si>
+  <si>
+    <t>Kyle</t>
+  </si>
+  <si>
+    <t>As UI engineer, I need a wireframe of the entire app.</t>
+  </si>
+  <si>
+    <t>Wayne</t>
+  </si>
+  <si>
+    <t>Khaled</t>
+  </si>
+  <si>
+    <t>Darren</t>
+  </si>
+  <si>
+    <t>As a developer, we need an algorithm for determining the performance metrics.</t>
+  </si>
+  <si>
+    <t>Ameer</t>
+  </si>
+  <si>
+    <t>As a UI designer, we need an app icon.</t>
+  </si>
+  <si>
+    <t>Rammy</t>
   </si>
 </sst>
 </file>
@@ -259,12 +304,63 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>69</xdr:row>
+      <xdr:row>73</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="1026" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12700000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 2" hidden="1"/>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -566,17 +662,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E48"/>
+  <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="162" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="162" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="66.5" customWidth="1"/>
-    <col min="2" max="2" width="35" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" customWidth="1"/>
     <col min="4" max="4" width="24.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -648,7 +744,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>18</v>
       </c>
@@ -664,7 +760,10 @@
         <v>20</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -675,154 +774,228 @@
         <v>22</v>
       </c>
       <c r="C16" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>31</v>
+      </c>
+      <c r="D16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>31</v>
+      </c>
+      <c r="D17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="B24" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C21" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="2" t="s">
+      <c r="B25" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="2" t="s">
+    </row>
+    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B26" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="2" t="s">
+    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B27" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="2" t="s">
+    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D28" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D31" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D32" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="2"/>
+    </row>
+    <row r="40" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A40" s="1"/>
+    </row>
+    <row r="41" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A41" s="4"/>
+    </row>
+    <row r="42" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A42" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="1" t="s">
+    </row>
+    <row r="43" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A43" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="2" t="s">
+    <row r="44" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A44" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="2" t="s">
+      <c r="B44" s="2"/>
+    </row>
+    <row r="45" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A45" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="2"/>
-    </row>
-    <row r="36" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="1"/>
-    </row>
-    <row r="37" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="4"/>
-    </row>
-    <row r="38" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="2"/>
-    </row>
-    <row r="39" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="2"/>
-    </row>
-    <row r="40" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="2"/>
-      <c r="B40" s="2"/>
-    </row>
-    <row r="41" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="2"/>
-      <c r="B41" s="2"/>
-    </row>
-    <row r="42" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="2"/>
-    </row>
-    <row r="43" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="2"/>
-      <c r="B43" s="2"/>
-    </row>
-    <row r="44" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="4"/>
-    </row>
-    <row r="45" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A45" s="2"/>
+      <c r="B45" s="2"/>
     </row>
     <row r="46" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="2"/>
     </row>
     <row r="47" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
     </row>
     <row r="48" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="2"/>
+      <c r="A48" s="4"/>
+    </row>
+    <row r="49" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A49" s="2"/>
+    </row>
+    <row r="50" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A50" s="2"/>
+    </row>
+    <row r="51" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A51" s="2"/>
+    </row>
+    <row r="52" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A52" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated the user stories
</commit_message>
<xml_diff>
--- a/Documents/Features & User Stories.xlsx
+++ b/Documents/Features & User Stories.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26606"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26812"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="66">
   <si>
     <t>Feature</t>
   </si>
@@ -220,25 +220,31 @@
     <t>As a developer, I need a user table so that we can track user information.</t>
   </si>
   <si>
-    <t xml:space="preserve">Kyle </t>
-  </si>
-  <si>
     <t>In progress</t>
   </si>
   <si>
     <t>Backlog</t>
   </si>
   <si>
-    <t>As a user, I need the performance tab to have a functional performance graph so that I can track my performance metrics.</t>
-  </si>
-  <si>
     <t>As a user, I need a create new note button,</t>
   </si>
   <si>
-    <t>As a user, I need a create note view, so that I can crete a note,</t>
+    <t>As a user I need a delete note button so that I can delete notes.</t>
   </si>
   <si>
-    <t>As a user I need a delete note button so that I can delete notes.</t>
+    <t>As a user, I need the progress bar changes to green when the task is at 100% completion so that I have an improved visual representation</t>
+  </si>
+  <si>
+    <t>Kahled</t>
+  </si>
+  <si>
+    <t>As a user, I need a create note view, so that I can create a new note</t>
+  </si>
+  <si>
+    <t>As a user , I need a performance graph on the performance tab, so that I can view performance data</t>
+  </si>
+  <si>
+    <t>As a user, I need the number of completed tasks, overdue tasks, and the average time tasks are late.</t>
   </si>
 </sst>
 </file>
@@ -304,7 +310,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -317,6 +323,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -400,6 +407,57 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12700000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>863600</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle 1" hidden="1"/>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -703,8 +761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B14" zoomScale="166" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="166" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1263,7 +1321,7 @@
         <v>30</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>26</v>
@@ -1407,7 +1465,7 @@
         <v>34</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -1513,7 +1571,7 @@
         <v>30</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -1619,7 +1677,7 @@
         <v>28</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>44</v>
@@ -1655,10 +1713,10 @@
         <v>28</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
@@ -1691,10 +1749,10 @@
         <v>28</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
@@ -1793,7 +1851,7 @@
     </row>
     <row r="33" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>28</v>
@@ -1827,7 +1885,7 @@
     </row>
     <row r="34" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="11" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B34" s="11" t="s">
         <v>28</v>
@@ -1838,7 +1896,7 @@
     </row>
     <row r="35" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>34</v>
@@ -1870,42 +1928,52 @@
       <c r="Y35" s="2"/>
       <c r="Z35" s="2"/>
     </row>
-    <row r="36" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
-      <c r="K36" s="2"/>
-      <c r="L36" s="2"/>
-      <c r="M36" s="2"/>
-      <c r="N36" s="2"/>
-      <c r="O36" s="2"/>
-      <c r="P36" s="2"/>
-      <c r="Q36" s="2"/>
-      <c r="R36" s="2"/>
-      <c r="S36" s="2"/>
-      <c r="T36" s="2"/>
-      <c r="U36" s="2"/>
-      <c r="V36" s="2"/>
-      <c r="W36" s="2"/>
-      <c r="X36" s="2"/>
-      <c r="Y36" s="2"/>
-      <c r="Z36" s="2"/>
+    <row r="36" spans="1:26" s="10" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="9"/>
+      <c r="J36" s="9"/>
+      <c r="K36" s="9"/>
+      <c r="L36" s="9"/>
+      <c r="M36" s="9"/>
+      <c r="N36" s="9"/>
+      <c r="O36" s="9"/>
+      <c r="P36" s="9"/>
+      <c r="Q36" s="9"/>
+      <c r="R36" s="9"/>
+      <c r="S36" s="9"/>
+      <c r="T36" s="9"/>
+      <c r="U36" s="9"/>
+      <c r="V36" s="9"/>
+      <c r="W36" s="9"/>
+      <c r="X36" s="9"/>
+      <c r="Y36" s="9"/>
+      <c r="Z36" s="9"/>
     </row>
     <row r="37" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="3" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C37" s="2"/>
+      <c r="C37" s="2" t="s">
+        <v>57</v>
+      </c>
       <c r="D37" s="6" t="s">
         <v>36</v>
       </c>
@@ -1933,10 +2001,18 @@
       <c r="Z37" s="2"/>
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
+      <c r="A38" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>36</v>
+      </c>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>

</xml_diff>

<commit_message>
Updated the user stories and roadmap.
</commit_message>
<xml_diff>
--- a/Documents/Features & User Stories.xlsx
+++ b/Documents/Features & User Stories.xlsx
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="65">
   <si>
     <t>Feature</t>
   </si>
@@ -193,9 +193,6 @@
     <t>As a developer, we need an algorithm for determining the performance metrics.</t>
   </si>
   <si>
-    <t>Pseudo Code Completed</t>
-  </si>
-  <si>
     <t>Ameer</t>
   </si>
   <si>
@@ -218,9 +215,6 @@
   </si>
   <si>
     <t>As a developer, I need a user table so that we can track user information.</t>
-  </si>
-  <si>
-    <t>In progress</t>
   </si>
   <si>
     <t>Backlog</t>
@@ -246,12 +240,15 @@
   <si>
     <t>As a user, I need the number of completed tasks, overdue tasks, and the average time tasks are late.</t>
   </si>
+  <si>
+    <t>Current goal: Polishing up the final version of the app.  Creating test cases.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -275,12 +272,6 @@
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -310,19 +301,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -350,7 +338,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>863600</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>64</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -401,7 +389,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>863600</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>64</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -452,12 +440,63 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>863600</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>64</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="3" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12700000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>863600</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectangle 1" hidden="1"/>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -759,10 +798,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="166" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="166" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1241,742 +1280,745 @@
       <c r="Y15" s="2"/>
       <c r="Z15" s="2"/>
     </row>
-    <row r="16" spans="1:26" s="10" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="8" t="s">
+    <row r="16" spans="1:26" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="9"/>
-      <c r="M16" s="9"/>
-      <c r="N16" s="9"/>
-      <c r="O16" s="9"/>
-      <c r="P16" s="9"/>
-      <c r="Q16" s="9"/>
-      <c r="R16" s="9"/>
-      <c r="S16" s="9"/>
-      <c r="T16" s="9"/>
-      <c r="U16" s="9"/>
-      <c r="V16" s="9"/>
-      <c r="W16" s="9"/>
-      <c r="X16" s="9"/>
-      <c r="Y16" s="9"/>
-      <c r="Z16" s="9"/>
-    </row>
-    <row r="17" spans="1:26" s="10" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="8" t="s">
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="7"/>
+      <c r="S16" s="7"/>
+      <c r="T16" s="7"/>
+      <c r="U16" s="7"/>
+      <c r="V16" s="7"/>
+      <c r="W16" s="7"/>
+      <c r="X16" s="7"/>
+      <c r="Y16" s="7"/>
+      <c r="Z16" s="7"/>
+    </row>
+    <row r="17" spans="1:26" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="9"/>
-      <c r="N17" s="9"/>
-      <c r="O17" s="9"/>
-      <c r="P17" s="9"/>
-      <c r="Q17" s="9"/>
-      <c r="R17" s="9"/>
-      <c r="S17" s="9"/>
-      <c r="T17" s="9"/>
-      <c r="U17" s="9"/>
-      <c r="V17" s="9"/>
-      <c r="W17" s="9"/>
-      <c r="X17" s="9"/>
-      <c r="Y17" s="9"/>
-      <c r="Z17" s="9"/>
-    </row>
-    <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="3" t="s">
-        <v>29</v>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7"/>
+      <c r="R17" s="7"/>
+      <c r="S17" s="7"/>
+      <c r="T17" s="7"/>
+      <c r="U17" s="7"/>
+      <c r="V17" s="7"/>
+      <c r="W17" s="7"/>
+      <c r="X17" s="7"/>
+      <c r="Y17" s="7"/>
+      <c r="Z17" s="7"/>
+    </row>
+    <row r="18" spans="1:26" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="6" t="s">
+        <v>31</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="7"/>
+      <c r="S18" s="7"/>
+      <c r="T18" s="7"/>
+      <c r="U18" s="7"/>
+      <c r="V18" s="7"/>
+      <c r="W18" s="7"/>
+      <c r="X18" s="7"/>
+      <c r="Y18" s="7"/>
+      <c r="Z18" s="7"/>
+    </row>
+    <row r="19" spans="1:26" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="7"/>
+      <c r="S19" s="7"/>
+      <c r="T19" s="7"/>
+      <c r="U19" s="7"/>
+      <c r="V19" s="7"/>
+      <c r="W19" s="7"/>
+      <c r="X19" s="7"/>
+      <c r="Y19" s="7"/>
+      <c r="Z19" s="7"/>
+    </row>
+    <row r="20" spans="1:26" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
+      <c r="R20" s="7"/>
+      <c r="S20" s="7"/>
+      <c r="T20" s="7"/>
+      <c r="U20" s="7"/>
+      <c r="V20" s="7"/>
+      <c r="W20" s="7"/>
+      <c r="X20" s="7"/>
+      <c r="Y20" s="7"/>
+      <c r="Z20" s="7"/>
+    </row>
+    <row r="21" spans="1:26" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7"/>
+      <c r="N21" s="7"/>
+      <c r="O21" s="7"/>
+      <c r="P21" s="7"/>
+      <c r="Q21" s="7"/>
+      <c r="R21" s="7"/>
+      <c r="S21" s="7"/>
+      <c r="T21" s="7"/>
+      <c r="U21" s="7"/>
+      <c r="V21" s="7"/>
+      <c r="W21" s="7"/>
+      <c r="X21" s="7"/>
+      <c r="Y21" s="7"/>
+      <c r="Z21" s="7"/>
+    </row>
+    <row r="22" spans="1:26" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="7"/>
+      <c r="N22" s="7"/>
+      <c r="O22" s="7"/>
+      <c r="P22" s="7"/>
+      <c r="Q22" s="7"/>
+      <c r="R22" s="7"/>
+      <c r="S22" s="7"/>
+      <c r="T22" s="7"/>
+      <c r="U22" s="7"/>
+      <c r="V22" s="7"/>
+      <c r="W22" s="7"/>
+      <c r="X22" s="7"/>
+      <c r="Y22" s="7"/>
+      <c r="Z22" s="7"/>
+    </row>
+    <row r="23" spans="1:26" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="7"/>
+      <c r="P23" s="7"/>
+      <c r="Q23" s="7"/>
+      <c r="R23" s="7"/>
+      <c r="S23" s="7"/>
+      <c r="T23" s="7"/>
+      <c r="U23" s="7"/>
+      <c r="V23" s="7"/>
+      <c r="W23" s="7"/>
+      <c r="X23" s="7"/>
+      <c r="Y23" s="7"/>
+      <c r="Z23" s="7"/>
+    </row>
+    <row r="24" spans="1:26" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="7"/>
+      <c r="P24" s="7"/>
+      <c r="Q24" s="7"/>
+      <c r="R24" s="7"/>
+      <c r="S24" s="7"/>
+      <c r="T24" s="7"/>
+      <c r="U24" s="7"/>
+      <c r="V24" s="7"/>
+      <c r="W24" s="7"/>
+      <c r="X24" s="7"/>
+      <c r="Y24" s="7"/>
+      <c r="Z24" s="7"/>
+    </row>
+    <row r="25" spans="1:26" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7"/>
+      <c r="N25" s="7"/>
+      <c r="O25" s="7"/>
+      <c r="P25" s="7"/>
+      <c r="Q25" s="7"/>
+      <c r="R25" s="7"/>
+      <c r="S25" s="7"/>
+      <c r="T25" s="7"/>
+      <c r="U25" s="7"/>
+      <c r="V25" s="7"/>
+      <c r="W25" s="7"/>
+      <c r="X25" s="7"/>
+      <c r="Y25" s="7"/>
+      <c r="Z25" s="7"/>
+    </row>
+    <row r="26" spans="1:26" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="7"/>
+      <c r="N26" s="7"/>
+      <c r="O26" s="7"/>
+      <c r="P26" s="7"/>
+      <c r="Q26" s="7"/>
+      <c r="R26" s="7"/>
+      <c r="S26" s="7"/>
+      <c r="T26" s="7"/>
+      <c r="U26" s="7"/>
+      <c r="V26" s="7"/>
+      <c r="W26" s="7"/>
+      <c r="X26" s="7"/>
+      <c r="Y26" s="7"/>
+      <c r="Z26" s="7"/>
+    </row>
+    <row r="27" spans="1:26" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="7"/>
+      <c r="N27" s="7"/>
+      <c r="O27" s="7"/>
+      <c r="P27" s="7"/>
+      <c r="Q27" s="7"/>
+      <c r="R27" s="7"/>
+      <c r="S27" s="7"/>
+      <c r="T27" s="7"/>
+      <c r="U27" s="7"/>
+      <c r="V27" s="7"/>
+      <c r="W27" s="7"/>
+      <c r="X27" s="7"/>
+      <c r="Y27" s="7"/>
+      <c r="Z27" s="7"/>
+    </row>
+    <row r="28" spans="1:26" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="7"/>
+      <c r="N28" s="7"/>
+      <c r="O28" s="7"/>
+      <c r="P28" s="7"/>
+      <c r="Q28" s="7"/>
+      <c r="R28" s="7"/>
+      <c r="S28" s="7"/>
+      <c r="T28" s="7"/>
+      <c r="U28" s="7"/>
+      <c r="V28" s="7"/>
+      <c r="W28" s="7"/>
+      <c r="X28" s="7"/>
+      <c r="Y28" s="7"/>
+      <c r="Z28" s="7"/>
+    </row>
+    <row r="29" spans="1:26" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
+      <c r="L29" s="7"/>
+      <c r="M29" s="7"/>
+      <c r="N29" s="7"/>
+      <c r="O29" s="7"/>
+      <c r="P29" s="7"/>
+      <c r="Q29" s="7"/>
+      <c r="R29" s="7"/>
+      <c r="S29" s="7"/>
+      <c r="T29" s="7"/>
+      <c r="U29" s="7"/>
+      <c r="V29" s="7"/>
+      <c r="W29" s="7"/>
+      <c r="X29" s="7"/>
+      <c r="Y29" s="7"/>
+      <c r="Z29" s="7"/>
+    </row>
+    <row r="30" spans="1:26" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="7"/>
+      <c r="L30" s="7"/>
+      <c r="M30" s="7"/>
+      <c r="N30" s="7"/>
+      <c r="O30" s="7"/>
+      <c r="P30" s="7"/>
+      <c r="Q30" s="7"/>
+      <c r="R30" s="7"/>
+      <c r="S30" s="7"/>
+      <c r="T30" s="7"/>
+      <c r="U30" s="7"/>
+      <c r="V30" s="7"/>
+      <c r="W30" s="7"/>
+      <c r="X30" s="7"/>
+      <c r="Y30" s="7"/>
+      <c r="Z30" s="7"/>
+    </row>
+    <row r="31" spans="1:26" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="7"/>
+      <c r="K31" s="7"/>
+      <c r="L31" s="7"/>
+      <c r="M31" s="7"/>
+      <c r="N31" s="7"/>
+      <c r="O31" s="7"/>
+      <c r="P31" s="7"/>
+      <c r="Q31" s="7"/>
+      <c r="R31" s="7"/>
+      <c r="S31" s="7"/>
+      <c r="T31" s="7"/>
+      <c r="U31" s="7"/>
+      <c r="V31" s="7"/>
+      <c r="W31" s="7"/>
+      <c r="X31" s="7"/>
+      <c r="Y31" s="7"/>
+      <c r="Z31" s="7"/>
+    </row>
+    <row r="32" spans="1:26" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="1:26" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="7"/>
+      <c r="M33" s="7"/>
+      <c r="N33" s="7"/>
+      <c r="O33" s="7"/>
+      <c r="P33" s="7"/>
+      <c r="Q33" s="7"/>
+      <c r="R33" s="7"/>
+      <c r="S33" s="7"/>
+      <c r="T33" s="7"/>
+      <c r="U33" s="7"/>
+      <c r="V33" s="7"/>
+      <c r="W33" s="7"/>
+      <c r="X33" s="7"/>
+      <c r="Y33" s="7"/>
+      <c r="Z33" s="7"/>
+    </row>
+    <row r="34" spans="1:26" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B34" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>58</v>
+      <c r="C34" s="7" t="s">
+        <v>25</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D34" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
-      <c r="P18" s="2"/>
-      <c r="Q18" s="2"/>
-      <c r="R18" s="2"/>
-      <c r="S18" s="2"/>
-      <c r="T18" s="2"/>
-      <c r="U18" s="2"/>
-      <c r="V18" s="2"/>
-      <c r="W18" s="2"/>
-      <c r="X18" s="2"/>
-      <c r="Y18" s="2"/>
-      <c r="Z18" s="2"/>
-    </row>
-    <row r="19" spans="1:26" s="10" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="8" t="s">
-        <v>31</v>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="7"/>
+      <c r="K34" s="7"/>
+      <c r="L34" s="7"/>
+      <c r="M34" s="7"/>
+      <c r="N34" s="7"/>
+      <c r="O34" s="7"/>
+      <c r="P34" s="7"/>
+      <c r="Q34" s="7"/>
+      <c r="R34" s="7"/>
+      <c r="S34" s="7"/>
+      <c r="T34" s="7"/>
+      <c r="U34" s="7"/>
+      <c r="V34" s="7"/>
+      <c r="W34" s="7"/>
+      <c r="X34" s="7"/>
+      <c r="Y34" s="7"/>
+      <c r="Z34" s="7"/>
+    </row>
+    <row r="35" spans="1:26" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="6" t="s">
+        <v>63</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B35" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C35" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="9" t="s">
-        <v>32</v>
+      <c r="D35" s="8" t="s">
+        <v>36</v>
       </c>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="9"/>
-      <c r="M19" s="9"/>
-      <c r="N19" s="9"/>
-      <c r="O19" s="9"/>
-      <c r="P19" s="9"/>
-      <c r="Q19" s="9"/>
-      <c r="R19" s="9"/>
-      <c r="S19" s="9"/>
-      <c r="T19" s="9"/>
-      <c r="U19" s="9"/>
-      <c r="V19" s="9"/>
-      <c r="W19" s="9"/>
-      <c r="X19" s="9"/>
-      <c r="Y19" s="9"/>
-      <c r="Z19" s="9"/>
-    </row>
-    <row r="20" spans="1:26" s="10" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="8" t="s">
-        <v>33</v>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="7"/>
+      <c r="K35" s="7"/>
+      <c r="L35" s="7"/>
+      <c r="M35" s="7"/>
+      <c r="N35" s="7"/>
+      <c r="O35" s="7"/>
+      <c r="P35" s="7"/>
+      <c r="Q35" s="7"/>
+      <c r="R35" s="7"/>
+      <c r="S35" s="7"/>
+      <c r="T35" s="7"/>
+      <c r="U35" s="7"/>
+      <c r="V35" s="7"/>
+      <c r="W35" s="7"/>
+      <c r="X35" s="7"/>
+      <c r="Y35" s="7"/>
+      <c r="Z35" s="7"/>
+    </row>
+    <row r="36" spans="1:26" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="6" t="s">
+        <v>62</v>
       </c>
-      <c r="B20" s="8" t="s">
-        <v>34</v>
+      <c r="B36" s="6" t="s">
+        <v>28</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C36" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="9"/>
-      <c r="N20" s="9"/>
-      <c r="O20" s="9"/>
-      <c r="P20" s="9"/>
-      <c r="Q20" s="9"/>
-      <c r="R20" s="9"/>
-      <c r="S20" s="9"/>
-      <c r="T20" s="9"/>
-      <c r="U20" s="9"/>
-      <c r="V20" s="9"/>
-      <c r="W20" s="9"/>
-      <c r="X20" s="9"/>
-      <c r="Y20" s="9"/>
-      <c r="Z20" s="9"/>
-    </row>
-    <row r="21" spans="1:26" s="10" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D21" s="9" t="s">
+      <c r="D36" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
-      <c r="L21" s="9"/>
-      <c r="M21" s="9"/>
-      <c r="N21" s="9"/>
-      <c r="O21" s="9"/>
-      <c r="P21" s="9"/>
-      <c r="Q21" s="9"/>
-      <c r="R21" s="9"/>
-      <c r="S21" s="9"/>
-      <c r="T21" s="9"/>
-      <c r="U21" s="9"/>
-      <c r="V21" s="9"/>
-      <c r="W21" s="9"/>
-      <c r="X21" s="9"/>
-      <c r="Y21" s="9"/>
-      <c r="Z21" s="9"/>
-    </row>
-    <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2"/>
-      <c r="O22" s="2"/>
-      <c r="P22" s="2"/>
-      <c r="Q22" s="2"/>
-      <c r="R22" s="2"/>
-      <c r="S22" s="2"/>
-      <c r="T22" s="2"/>
-      <c r="U22" s="2"/>
-      <c r="V22" s="2"/>
-      <c r="W22" s="2"/>
-      <c r="X22" s="2"/>
-      <c r="Y22" s="2"/>
-      <c r="Z22" s="2"/>
-    </row>
-    <row r="23" spans="1:26" s="10" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
-      <c r="L23" s="9"/>
-      <c r="M23" s="9"/>
-      <c r="N23" s="9"/>
-      <c r="O23" s="9"/>
-      <c r="P23" s="9"/>
-      <c r="Q23" s="9"/>
-      <c r="R23" s="9"/>
-      <c r="S23" s="9"/>
-      <c r="T23" s="9"/>
-      <c r="U23" s="9"/>
-      <c r="V23" s="9"/>
-      <c r="W23" s="9"/>
-      <c r="X23" s="9"/>
-      <c r="Y23" s="9"/>
-      <c r="Z23" s="9"/>
-    </row>
-    <row r="24" spans="1:26" s="10" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="9"/>
-      <c r="L24" s="9"/>
-      <c r="M24" s="9"/>
-      <c r="N24" s="9"/>
-      <c r="O24" s="9"/>
-      <c r="P24" s="9"/>
-      <c r="Q24" s="9"/>
-      <c r="R24" s="9"/>
-      <c r="S24" s="9"/>
-      <c r="T24" s="9"/>
-      <c r="U24" s="9"/>
-      <c r="V24" s="9"/>
-      <c r="W24" s="9"/>
-      <c r="X24" s="9"/>
-      <c r="Y24" s="9"/>
-      <c r="Z24" s="9"/>
-    </row>
-    <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
-      <c r="L25" s="2"/>
-      <c r="M25" s="2"/>
-      <c r="N25" s="2"/>
-      <c r="O25" s="2"/>
-      <c r="P25" s="2"/>
-      <c r="Q25" s="2"/>
-      <c r="R25" s="2"/>
-      <c r="S25" s="2"/>
-      <c r="T25" s="2"/>
-      <c r="U25" s="2"/>
-      <c r="V25" s="2"/>
-      <c r="W25" s="2"/>
-      <c r="X25" s="2"/>
-      <c r="Y25" s="2"/>
-      <c r="Z25" s="2"/>
-    </row>
-    <row r="26" spans="1:26" s="10" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="9"/>
-      <c r="J26" s="9"/>
-      <c r="K26" s="9"/>
-      <c r="L26" s="9"/>
-      <c r="M26" s="9"/>
-      <c r="N26" s="9"/>
-      <c r="O26" s="9"/>
-      <c r="P26" s="9"/>
-      <c r="Q26" s="9"/>
-      <c r="R26" s="9"/>
-      <c r="S26" s="9"/>
-      <c r="T26" s="9"/>
-      <c r="U26" s="9"/>
-      <c r="V26" s="9"/>
-      <c r="W26" s="9"/>
-      <c r="X26" s="9"/>
-      <c r="Y26" s="9"/>
-      <c r="Z26" s="9"/>
-    </row>
-    <row r="27" spans="1:26" s="10" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="9"/>
-      <c r="J27" s="9"/>
-      <c r="K27" s="9"/>
-      <c r="L27" s="9"/>
-      <c r="M27" s="9"/>
-      <c r="N27" s="9"/>
-      <c r="O27" s="9"/>
-      <c r="P27" s="9"/>
-      <c r="Q27" s="9"/>
-      <c r="R27" s="9"/>
-      <c r="S27" s="9"/>
-      <c r="T27" s="9"/>
-      <c r="U27" s="9"/>
-      <c r="V27" s="9"/>
-      <c r="W27" s="9"/>
-      <c r="X27" s="9"/>
-      <c r="Y27" s="9"/>
-      <c r="Z27" s="9"/>
-    </row>
-    <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
-      <c r="L28" s="2"/>
-      <c r="M28" s="2"/>
-      <c r="N28" s="2"/>
-      <c r="O28" s="2"/>
-      <c r="P28" s="2"/>
-      <c r="Q28" s="2"/>
-      <c r="R28" s="2"/>
-      <c r="S28" s="2"/>
-      <c r="T28" s="2"/>
-      <c r="U28" s="2"/>
-      <c r="V28" s="2"/>
-      <c r="W28" s="2"/>
-      <c r="X28" s="2"/>
-      <c r="Y28" s="2"/>
-      <c r="Z28" s="2"/>
-    </row>
-    <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
-      <c r="L29" s="2"/>
-      <c r="M29" s="2"/>
-      <c r="N29" s="2"/>
-      <c r="O29" s="2"/>
-      <c r="P29" s="2"/>
-      <c r="Q29" s="2"/>
-      <c r="R29" s="2"/>
-      <c r="S29" s="2"/>
-      <c r="T29" s="2"/>
-      <c r="U29" s="2"/>
-      <c r="V29" s="2"/>
-      <c r="W29" s="2"/>
-      <c r="X29" s="2"/>
-      <c r="Y29" s="2"/>
-      <c r="Z29" s="2"/>
-    </row>
-    <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
-      <c r="L30" s="2"/>
-      <c r="M30" s="2"/>
-      <c r="N30" s="2"/>
-      <c r="O30" s="2"/>
-      <c r="P30" s="2"/>
-      <c r="Q30" s="2"/>
-      <c r="R30" s="2"/>
-      <c r="S30" s="2"/>
-      <c r="T30" s="2"/>
-      <c r="U30" s="2"/>
-      <c r="V30" s="2"/>
-      <c r="W30" s="2"/>
-      <c r="X30" s="2"/>
-      <c r="Y30" s="2"/>
-      <c r="Z30" s="2"/>
-    </row>
-    <row r="31" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
-      <c r="L31" s="2"/>
-      <c r="M31" s="2"/>
-      <c r="N31" s="2"/>
-      <c r="O31" s="2"/>
-      <c r="P31" s="2"/>
-      <c r="Q31" s="2"/>
-      <c r="R31" s="2"/>
-      <c r="S31" s="2"/>
-      <c r="T31" s="2"/>
-      <c r="U31" s="2"/>
-      <c r="V31" s="2"/>
-      <c r="W31" s="2"/>
-      <c r="X31" s="2"/>
-      <c r="Y31" s="2"/>
-      <c r="Z31" s="2"/>
-    </row>
-    <row r="32" spans="1:26" s="10" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="B32" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D32" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="9"/>
-      <c r="I32" s="9"/>
-      <c r="J32" s="9"/>
-      <c r="K32" s="9"/>
-      <c r="L32" s="9"/>
-      <c r="M32" s="9"/>
-      <c r="N32" s="9"/>
-      <c r="O32" s="9"/>
-      <c r="P32" s="9"/>
-      <c r="Q32" s="9"/>
-      <c r="R32" s="9"/>
-      <c r="S32" s="9"/>
-      <c r="T32" s="9"/>
-      <c r="U32" s="9"/>
-      <c r="V32" s="9"/>
-      <c r="W32" s="9"/>
-      <c r="X32" s="9"/>
-      <c r="Y32" s="9"/>
-      <c r="Z32" s="9"/>
-    </row>
-    <row r="33" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C33" s="2"/>
-      <c r="D33" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
-      <c r="L33" s="2"/>
-      <c r="M33" s="2"/>
-      <c r="N33" s="2"/>
-      <c r="O33" s="2"/>
-      <c r="P33" s="2"/>
-      <c r="Q33" s="2"/>
-      <c r="R33" s="2"/>
-      <c r="S33" s="2"/>
-      <c r="T33" s="2"/>
-      <c r="U33" s="2"/>
-      <c r="V33" s="2"/>
-      <c r="W33" s="2"/>
-      <c r="X33" s="2"/>
-      <c r="Y33" s="2"/>
-      <c r="Z33" s="2"/>
-    </row>
-    <row r="34" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="B34" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="35" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C35" s="2"/>
-      <c r="D35" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
-      <c r="K35" s="2"/>
-      <c r="L35" s="2"/>
-      <c r="M35" s="2"/>
-      <c r="N35" s="2"/>
-      <c r="O35" s="2"/>
-      <c r="P35" s="2"/>
-      <c r="Q35" s="2"/>
-      <c r="R35" s="2"/>
-      <c r="S35" s="2"/>
-      <c r="T35" s="2"/>
-      <c r="U35" s="2"/>
-      <c r="V35" s="2"/>
-      <c r="W35" s="2"/>
-      <c r="X35" s="2"/>
-      <c r="Y35" s="2"/>
-      <c r="Z35" s="2"/>
-    </row>
-    <row r="36" spans="1:26" s="10" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D36" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="E36" s="9"/>
-      <c r="F36" s="9"/>
-      <c r="G36" s="9"/>
-      <c r="H36" s="9"/>
-      <c r="I36" s="9"/>
-      <c r="J36" s="9"/>
-      <c r="K36" s="9"/>
-      <c r="L36" s="9"/>
-      <c r="M36" s="9"/>
-      <c r="N36" s="9"/>
-      <c r="O36" s="9"/>
-      <c r="P36" s="9"/>
-      <c r="Q36" s="9"/>
-      <c r="R36" s="9"/>
-      <c r="S36" s="9"/>
-      <c r="T36" s="9"/>
-      <c r="U36" s="9"/>
-      <c r="V36" s="9"/>
-      <c r="W36" s="9"/>
-      <c r="X36" s="9"/>
-      <c r="Y36" s="9"/>
-      <c r="Z36" s="9"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="7"/>
+      <c r="K36" s="7"/>
+      <c r="L36" s="7"/>
+      <c r="M36" s="7"/>
+      <c r="N36" s="7"/>
+      <c r="O36" s="7"/>
+      <c r="P36" s="7"/>
+      <c r="Q36" s="7"/>
+      <c r="R36" s="7"/>
+      <c r="S36" s="7"/>
+      <c r="T36" s="7"/>
+      <c r="U36" s="7"/>
+      <c r="V36" s="7"/>
+      <c r="W36" s="7"/>
+      <c r="X36" s="7"/>
+      <c r="Y36" s="7"/>
+      <c r="Z36" s="7"/>
     </row>
     <row r="37" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>36</v>
-      </c>
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
@@ -2002,17 +2044,15 @@
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="3" t="s">
-        <v>64</v>
+        <v>29</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
-      <c r="D38" s="6" t="s">
-        <v>36</v>
-      </c>
+      <c r="D38" s="2"/>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
@@ -2037,9 +2077,15 @@
       <c r="Z38" s="2"/>
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
+      <c r="A39" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
@@ -2065,7 +2111,6 @@
       <c r="Z39" s="2"/>
     </row>
     <row r="40" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="1"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
@@ -2093,7 +2138,9 @@
       <c r="Z40" s="2"/>
     </row>
     <row r="41" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="7"/>
+      <c r="A41" t="s">
+        <v>64</v>
+      </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
@@ -2121,10 +2168,7 @@
       <c r="Z41" s="2"/>
     </row>
     <row r="42" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B42" s="2"/>
+      <c r="B42" s="3"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
@@ -2151,10 +2195,7 @@
       <c r="Z42" s="2"/>
     </row>
     <row r="43" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B43" s="2"/>
+      <c r="B43" s="3"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
@@ -2181,10 +2222,8 @@
       <c r="Z43" s="2"/>
     </row>
     <row r="44" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B44" s="3"/>
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
@@ -2211,10 +2250,10 @@
       <c r="Z44" s="2"/>
     </row>
     <row r="45" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A45" s="3" t="s">
-        <v>56</v>
+      <c r="A45" s="1" t="s">
+        <v>52</v>
       </c>
-      <c r="B45" s="3"/>
+      <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
@@ -2241,7 +2280,9 @@
       <c r="Z45" s="2"/>
     </row>
     <row r="46" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="2"/>
+      <c r="A46" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
@@ -2269,7 +2310,9 @@
       <c r="Z46" s="2"/>
     </row>
     <row r="47" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="2"/>
+      <c r="A47" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
@@ -2297,7 +2340,9 @@
       <c r="Z47" s="2"/>
     </row>
     <row r="48" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="2"/>
+      <c r="A48" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
@@ -28924,62 +28969,6 @@
       <c r="Y998" s="2"/>
       <c r="Z998" s="2"/>
     </row>
-    <row r="999" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A999" s="2"/>
-      <c r="B999" s="2"/>
-      <c r="C999" s="2"/>
-      <c r="D999" s="2"/>
-      <c r="E999" s="2"/>
-      <c r="F999" s="2"/>
-      <c r="G999" s="2"/>
-      <c r="H999" s="2"/>
-      <c r="I999" s="2"/>
-      <c r="J999" s="2"/>
-      <c r="K999" s="2"/>
-      <c r="L999" s="2"/>
-      <c r="M999" s="2"/>
-      <c r="N999" s="2"/>
-      <c r="O999" s="2"/>
-      <c r="P999" s="2"/>
-      <c r="Q999" s="2"/>
-      <c r="R999" s="2"/>
-      <c r="S999" s="2"/>
-      <c r="T999" s="2"/>
-      <c r="U999" s="2"/>
-      <c r="V999" s="2"/>
-      <c r="W999" s="2"/>
-      <c r="X999" s="2"/>
-      <c r="Y999" s="2"/>
-      <c r="Z999" s="2"/>
-    </row>
-    <row r="1000" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1000" s="2"/>
-      <c r="B1000" s="2"/>
-      <c r="C1000" s="2"/>
-      <c r="D1000" s="2"/>
-      <c r="E1000" s="2"/>
-      <c r="F1000" s="2"/>
-      <c r="G1000" s="2"/>
-      <c r="H1000" s="2"/>
-      <c r="I1000" s="2"/>
-      <c r="J1000" s="2"/>
-      <c r="K1000" s="2"/>
-      <c r="L1000" s="2"/>
-      <c r="M1000" s="2"/>
-      <c r="N1000" s="2"/>
-      <c r="O1000" s="2"/>
-      <c r="P1000" s="2"/>
-      <c r="Q1000" s="2"/>
-      <c r="R1000" s="2"/>
-      <c r="S1000" s="2"/>
-      <c r="T1000" s="2"/>
-      <c r="U1000" s="2"/>
-      <c r="V1000" s="2"/>
-      <c r="W1000" s="2"/>
-      <c r="X1000" s="2"/>
-      <c r="Y1000" s="2"/>
-      <c r="Z1000" s="2"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>